<commit_message>
Tuning simulation to change on/off temperature. Then making the resulting changes to BoM
</commit_message>
<xml_diff>
--- a/hardware/uob-hep-pc068a-cryosub/cryosub_top_v01/cryosub_top_v01.xlsx
+++ b/hardware/uob-hep-pc068a-cryosub/cryosub_top_v01/cryosub_top_v01.xlsx
@@ -125,7 +125,7 @@
     <t xml:space="preserve">10k Thermistor_NTC</t>
   </si>
   <si>
-    <t xml:space="preserve">Farnell 2432569</t>
+    <t xml:space="preserve">RS 525-9235</t>
   </si>
   <si>
     <t xml:space="preserve">Mitsubishi TH20-3H103FB Thermistor, 0805 (2012M) 10kΩ, 2 x 1.25 x 1.25mm</t>
@@ -312,12 +312,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -365,17 +361,17 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.28"/>
   </cols>
@@ -410,21 +406,21 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
       <c r="K2" s="0" t="s">
         <v>11</v>
       </c>
@@ -433,21 +429,21 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
       <c r="K3" s="0" t="s">
         <v>11</v>
       </c>
@@ -456,21 +452,21 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="K4" s="0" t="s">
         <v>11</v>
       </c>
@@ -479,21 +475,21 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="K5" s="0" t="s">
         <v>11</v>
       </c>
@@ -502,23 +498,23 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
       <c r="K6" s="0" t="s">
         <v>11</v>
       </c>
@@ -527,67 +523,67 @@
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="1"/>
       <c r="K9" s="0" t="s">
         <v>11</v>
       </c>
@@ -596,25 +592,25 @@
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="1"/>
       <c r="K10" s="0" t="s">
         <v>11</v>
       </c>
@@ -623,25 +619,25 @@
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="1"/>
       <c r="K11" s="0" t="s">
         <v>11</v>
       </c>
@@ -650,143 +646,143 @@
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
       <c r="K18" s="0" t="s">
         <v>11</v>
       </c>
@@ -795,23 +791,23 @@
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>61</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="K19" s="0" t="s">
         <v>11</v>
       </c>
@@ -820,43 +816,43 @@
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
       <c r="K21" s="0" t="s">
         <v>11</v>
       </c>
@@ -886,7 +882,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>